<commit_message>
Made Timeslot code working
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitchel\Documents\TU\AE4441-16 Operations optimisation\Assignment\OperationsOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A418CEAC-B8B6-420F-82DB-BF7F4EEE6A9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF15896-2595-42F2-9A99-247177B5F876}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8388" yWindow="1596" windowWidth="11256" windowHeight="8844" firstSheet="2" activeTab="3" xr2:uid="{57C2F7B5-A351-4D82-8024-C593F424B15D}"/>
+    <workbookView xWindow="9180" yWindow="1656" windowWidth="11256" windowHeight="8844" firstSheet="4" activeTab="4" xr2:uid="{57C2F7B5-A351-4D82-8024-C593F424B15D}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
     <sheet name="Time_interval" sheetId="2" r:id="rId2"/>
     <sheet name="Blad3" sheetId="3" r:id="rId3"/>
     <sheet name="new_dataset" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">Model!$P$8:$AE$8</definedName>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>Flight</t>
   </si>
@@ -185,18 +186,6 @@
   </si>
   <si>
     <t>Gate_com</t>
-  </si>
-  <si>
-    <t>1,2,3</t>
-  </si>
-  <si>
-    <t>3,4,5</t>
-  </si>
-  <si>
-    <t>3,4,6</t>
-  </si>
-  <si>
-    <t>1,2,4</t>
   </si>
 </sst>
 </file>
@@ -564,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A43E037-5129-47AC-AB25-5390A36FF942}">
   <dimension ref="A1:AH61"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2890,10 +2879,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A265F2-913F-4995-9AD1-C3D93AF37EF1}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection sqref="A1:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2901,128 +2890,623 @@
     <col min="2" max="2" width="11.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="1">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
         <v>0.38541666666666669</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F2" s="1">
         <v>0.41666666666666669</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
         <v>0.40625</v>
       </c>
-      <c r="D3" s="1">
+      <c r="F6" s="1">
         <v>0.46875</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="1">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D4" s="1">
+      <c r="F10" s="1">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="1">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D5" s="1">
+      <c r="F11" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F14" s="1">
         <v>0.51041666666666663</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
         <v>0.48958333333333331</v>
       </c>
-      <c r="D6" s="1">
+      <c r="F18" s="1">
         <v>0.54166666666666663</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>5</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.54166666666666663</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED46809A-AE24-43B9-8F63-9143E85F558D}">
+  <dimension ref="A1:F21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.40625</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.46875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.51041666666666663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added t variables and transfers
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daam\Documents\OpOp_assignment\OperationsOptimization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitchel\Documents\TU\AE4441-16 Operations optimisation\Assignment\OperationsOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257F02FD-30F9-4469-A71B-0B82CDD57C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46C41BC-E902-49CE-BCC9-730B8C45E486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="4" xr2:uid="{57C2F7B5-A351-4D82-8024-C593F424B15D}"/>
   </bookViews>
@@ -54,10 +54,18 @@
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -220,7 +228,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +238,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -261,15 +277,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -282,8 +324,32 @@
 </styleSheet>
 </file>
 
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41C64F55-0EB1-4F1E-977C-15A030BFD2F4}" name="Table1" displayName="Table1" ref="A1:O7" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:O7" xr:uid="{6F407DF8-F1E5-4646-87A7-4A6D757BAA65}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{35AA84A0-17ED-488D-BD75-42A9A1A9D6A4}" name="Flight"/>
+    <tableColumn id="2" xr3:uid="{C3E02A15-66CC-47E2-90FC-79E43FA4A71D}" name="Passengers"/>
+    <tableColumn id="3" xr3:uid="{CDCEC883-9402-444D-B0A6-D9AD2FE8CD50}" name="arr_time" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{F2766B2E-49BD-4B5C-94CB-4711EC7C0F1F}" name="dep_time" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{C34B4F9B-F41C-4458-A4D5-106757CBDD90}" name="Gate 1"/>
+    <tableColumn id="6" xr3:uid="{C9EE310D-5943-4A77-9638-90D6332A6440}" name="Gate 2"/>
+    <tableColumn id="7" xr3:uid="{71937E98-F077-4897-91A9-F0A4FAB0A02D}" name="Gate 3"/>
+    <tableColumn id="8" xr3:uid="{DC750559-06BF-4CB7-BAD4-D8F99CD72519}" name="Gate 4"/>
+    <tableColumn id="9" xr3:uid="{1E8E33B4-3F2F-4186-8466-26724C5554A7}" name="Gate 5"/>
+    <tableColumn id="10" xr3:uid="{78FA99B6-3F71-4049-98AC-A52435E42B11}" name="Flight 1 "/>
+    <tableColumn id="11" xr3:uid="{857450EF-EFF8-4421-B82F-B2CCEC68C563}" name="Flight 2 "/>
+    <tableColumn id="12" xr3:uid="{FF65540F-6929-48A1-8D94-D4B616D2FEDF}" name="Flight 3 "/>
+    <tableColumn id="13" xr3:uid="{8B2BCFF8-38CE-489F-B092-D0ED1B3E8DA7}" name="Flight 4 "/>
+    <tableColumn id="14" xr3:uid="{0A0F83E7-9ACB-483E-8CE7-CD810DDFE7AC}" name="Flight 5"/>
+    <tableColumn id="15" xr3:uid="{87ED476B-0C21-4266-8750-A157D4BAA274}" name="Flight 6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3348,61 +3414,65 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED46809A-AE24-43B9-8F63-9143E85F558D}">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" customWidth="1"/>
+    <col min="10" max="10" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="3" t="s">
         <v>49</v>
       </c>
     </row>
@@ -3411,7 +3481,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="C2" s="1">
         <v>0.38541666666666669</v>
@@ -3426,13 +3496,31 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>50</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>40</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -3440,7 +3528,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="C3" s="1">
         <v>0.40625</v>
@@ -3455,13 +3543,31 @@
         <v>2</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>20</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
@@ -3469,7 +3575,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="C4" s="1">
         <v>0.45833333333333331</v>
@@ -3481,16 +3587,34 @@
         <v>0</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -3498,7 +3622,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>180</v>
       </c>
       <c r="C5" s="1">
         <v>0.45833333333333331</v>
@@ -3507,19 +3631,37 @@
         <v>0.51041666666666663</v>
       </c>
       <c r="E5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H5">
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>30</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -3527,7 +3669,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>270</v>
       </c>
       <c r="C6" s="1">
         <v>0.48958333333333331</v>
@@ -3545,9 +3687,27 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2">
+        <v>0</v>
+      </c>
+      <c r="O6">
         <v>0</v>
       </c>
     </row>
@@ -3556,7 +3716,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1</v>
+        <v>320</v>
       </c>
       <c r="C7" s="1">
         <v>0.55555555555555558</v>
@@ -3565,18 +3725,36 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F7">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="2">
         <v>0</v>
       </c>
     </row>
@@ -3626,5 +3804,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added buffertime to model
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mitchel\Documents\TU\AE4441-16 Operations optimisation\Assignment\OperationsOptimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBACF295-ADD4-4439-80C5-00F4B3D60539}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF30877C-771F-4A80-825F-17470461545A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="2388" windowWidth="11256" windowHeight="8844" firstSheet="4" activeTab="4" xr2:uid="{57C2F7B5-A351-4D82-8024-C593F424B15D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="4" xr2:uid="{57C2F7B5-A351-4D82-8024-C593F424B15D}"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -231,6 +231,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -280,16 +283,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -308,12 +318,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -328,13 +332,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41C64F55-0EB1-4F1E-977C-15A030BFD2F4}" name="Table1" displayName="Table1" ref="A1:O7" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41C64F55-0EB1-4F1E-977C-15A030BFD2F4}" name="Table1" displayName="Table1" ref="A1:O7" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:O7" xr:uid="{6F407DF8-F1E5-4646-87A7-4A6D757BAA65}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{35AA84A0-17ED-488D-BD75-42A9A1A9D6A4}" name="Flights"/>
     <tableColumn id="2" xr3:uid="{C3E02A15-66CC-47E2-90FC-79E43FA4A71D}" name="Passengers"/>
-    <tableColumn id="3" xr3:uid="{CDCEC883-9402-444D-B0A6-D9AD2FE8CD50}" name="arr_time" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{F2766B2E-49BD-4B5C-94CB-4711EC7C0F1F}" name="dep_time" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{CDCEC883-9402-444D-B0A6-D9AD2FE8CD50}" name="arr_time" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{F2766B2E-49BD-4B5C-94CB-4711EC7C0F1F}" name="dep_time" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{C34B4F9B-F41C-4458-A4D5-106757CBDD90}" name="Gate 1"/>
     <tableColumn id="6" xr3:uid="{C9EE310D-5943-4A77-9638-90D6332A6440}" name="Gate 2"/>
     <tableColumn id="7" xr3:uid="{71937E98-F077-4897-91A9-F0A4FAB0A02D}" name="Gate 3"/>
@@ -3418,7 +3422,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3486,10 +3490,10 @@
       <c r="B2">
         <v>100</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="4">
         <v>0.38541666666666669</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="4">
         <v>0.41666666666666669</v>
       </c>
       <c r="E2">
@@ -3533,10 +3537,10 @@
       <c r="B3">
         <v>100</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="4">
         <v>0.40625</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="4">
         <v>0.46875</v>
       </c>
       <c r="E3">
@@ -3580,11 +3584,11 @@
       <c r="B4">
         <v>100</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D4" s="1">
-        <v>0.4861111111111111</v>
+      <c r="D4" s="4">
+        <v>0.49652777777777773</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3627,10 +3631,10 @@
       <c r="B5">
         <v>100</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="4">
         <v>0.45833333333333331</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="4">
         <v>0.51041666666666663</v>
       </c>
       <c r="E5">
@@ -3674,10 +3678,10 @@
       <c r="B6">
         <v>100</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="4">
         <v>0.48958333333333331</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="4">
         <v>0.54166666666666663</v>
       </c>
       <c r="E6">
@@ -3721,10 +3725,10 @@
       <c r="B7">
         <v>100</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="4">
         <v>0.55555555555555558</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="4">
         <v>0.58333333333333337</v>
       </c>
       <c r="E7">

</xml_diff>